<commit_message>
Fixed data git add .
</commit_message>
<xml_diff>
--- a/cypress/fixtures/credentials.xlsx
+++ b/cypress/fixtures/credentials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prita\Downloads\Compressed\Cypress_JS_POM-Allure-25.2-07-23\Jira-Automation-Cypress\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Fiverr Project\Project\Jira-Cypress-JS-Data-Driven\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B66A8B9-1C83-4EEA-870F-D76A6EE7ADF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554DA48B-99DF-41E5-AC64-A743486B5E0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{1324497D-A6C1-42B5-A9BE-66B3601190DC}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>user</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>psluzsvajnplxbupyt@cazlv.com</t>
-  </si>
-  <si>
-    <t>E2ETesting@123</t>
   </si>
 </sst>
 </file>
@@ -402,7 +396,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,18 +415,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7D2F532D-A240-4EBC-AD65-B31F97B7563D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>